<commit_message>
fixed the correlations; commented traffic_stats; add states coding file
</commit_message>
<xml_diff>
--- a/kc/state.xlsx
+++ b/kc/state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\Classes\W210 - Capstone\NYCTrafficCollisions\kc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D191BBB1-20E5-4123-8A72-7E375F6A28EF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEC2E01-94A7-4B46-8425-E1A4EF6FF8E4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11880" xr2:uid="{895920F2-0ACD-4D32-AD79-F578399110C0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Alabama</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -562,505 +568,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9365692-8FA0-41B7-A0F4-E70681428C73}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
+        <v>98</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>99</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>